<commit_message>
Retune first 2 missions
</commit_message>
<xml_diff>
--- a/dev/docs/loot.xlsx
+++ b/dev/docs/loot.xlsx
@@ -1,17 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{E4AFDE9A-B756-4BC6-84B5-9D17CE9B4A0C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Equipment" sheetId="1" r:id="rId1"/>
     <sheet name="Spells" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="54">
   <si>
     <t>Mage Level 1</t>
   </si>
@@ -180,12 +179,15 @@
   </si>
   <si>
     <t>HQ box</t>
+  </si>
+  <si>
+    <t>Warehouse</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -489,45 +491,45 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FD739F4-2923-42F4-8592-3E03BABFACD5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="13.90625" customWidth="1"/>
-    <col min="3" max="3" width="14.6328125" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -538,12 +540,12 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -551,12 +553,12 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -564,30 +566,33 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -595,197 +600,197 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:1" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:1" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:1" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:1" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:1" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:1" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:1" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:1" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:1" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:1" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:1" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:1" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:1" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:1" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:1" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:1" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:1" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:1" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:1" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:1" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:1" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:1" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:1" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:1" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:1" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:1" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>50</v>
       </c>

</xml_diff>

<commit_message>
Work on Nighttime event and Timon areas
</commit_message>
<xml_diff>
--- a/dev/docs/loot.xlsx
+++ b/dev/docs/loot.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="56">
   <si>
     <t>Mage Level 1</t>
   </si>
@@ -182,6 +182,12 @@
   </si>
   <si>
     <t>Warehouse</t>
+  </si>
+  <si>
+    <t>Skyflow -&gt; 4F -&gt; Main Hall</t>
+  </si>
+  <si>
+    <t>Human Resource basement</t>
   </si>
 </sst>
 </file>
@@ -514,7 +520,7 @@
   <dimension ref="A1:C53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -549,9 +555,6 @@
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
-        <v>52</v>
-      </c>
     </row>
     <row r="5" spans="1:3" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -565,11 +568,17 @@
       <c r="B6" t="s">
         <v>51</v>
       </c>
+      <c r="C6" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="7" spans="1:3" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>6</v>
       </c>
+      <c r="B7" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="8" spans="1:3" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
@@ -613,6 +622,9 @@
     <row r="14" spans="1:3" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="14.45" x14ac:dyDescent="0.35">

</xml_diff>